<commit_message>
Auto stash before merge of "master" and "Praktikum4/master"
</commit_message>
<xml_diff>
--- a/523/data/friedrich.xlsx
+++ b/523/data/friedrich.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Stuff" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>n</t>
   </si>
@@ -54,13 +54,16 @@
     <t>dN</t>
   </si>
   <si>
-    <t>Nunter</t>
-  </si>
-  <si>
     <t>N/40s</t>
   </si>
   <si>
     <t>dN/40s</t>
+  </si>
+  <si>
+    <t>dNunten</t>
+  </si>
+  <si>
+    <t>Nunten</t>
   </si>
 </sst>
 </file>
@@ -1901,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,10 +1927,10 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
         <v>12</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
@@ -2752,15 +2755,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:H25"/>
+  <dimension ref="C4:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -2777,10 +2780,13 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>40</v>
       </c>
@@ -2795,11 +2801,15 @@
         <v>7.745966692414834</v>
       </c>
       <c r="H5">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I5">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>40</v>
       </c>
@@ -2814,11 +2824,15 @@
         <v>6.7082039324993694</v>
       </c>
       <c r="H6">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I6">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>26</v>
       </c>
@@ -2830,11 +2844,15 @@
         <v>7.0710678118654755</v>
       </c>
       <c r="H7">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I7">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>32.1</v>
       </c>
@@ -2846,11 +2864,15 @@
         <v>6.6332495807107996</v>
       </c>
       <c r="H8">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I8">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>40.1</v>
       </c>
@@ -2862,11 +2884,15 @@
         <v>6</v>
       </c>
       <c r="H9">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I9">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>48.1</v>
       </c>
@@ -2878,11 +2904,15 @@
         <v>6.8556546004010439</v>
       </c>
       <c r="H10">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I10">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>56.2</v>
       </c>
@@ -2894,11 +2924,15 @@
         <v>7.3484692283495345</v>
       </c>
       <c r="H11">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I11">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>64.3</v>
       </c>
@@ -2910,11 +2944,15 @@
         <v>9.1651513899116797</v>
       </c>
       <c r="H12">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I12">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>72.400000000000006</v>
       </c>
@@ -2926,11 +2964,15 @@
         <v>11.532562594670797</v>
       </c>
       <c r="H13">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I13">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>80</v>
       </c>
@@ -2942,11 +2984,15 @@
         <v>14.142135623730951</v>
       </c>
       <c r="H14">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I14">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>88.1</v>
       </c>
@@ -2958,11 +3004,15 @@
         <v>14.866068747318506</v>
       </c>
       <c r="H15">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I15">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>96.3</v>
       </c>
@@ -2974,11 +3024,15 @@
         <v>14.730919862656235</v>
       </c>
       <c r="H16">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I16">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E17">
         <v>104</v>
       </c>
@@ -2990,11 +3044,15 @@
         <v>16.124515496597098</v>
       </c>
       <c r="H17">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I17">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>112</v>
       </c>
@@ -3006,11 +3064,15 @@
         <v>14.212670403551895</v>
       </c>
       <c r="H18">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I18">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>120</v>
       </c>
@@ -3022,11 +3084,15 @@
         <v>14.071247279470288</v>
       </c>
       <c r="H19">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I19">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>128</v>
       </c>
@@ -3038,11 +3104,15 @@
         <v>12.489995996796797</v>
       </c>
       <c r="H20">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I20">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>135.9</v>
       </c>
@@ -3054,11 +3124,15 @@
         <v>11.661903789690601</v>
       </c>
       <c r="H21">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I21">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>143.9</v>
       </c>
@@ -3070,11 +3144,15 @@
         <v>10.488088481701515</v>
       </c>
       <c r="H22">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I22">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>151.9</v>
       </c>
@@ -3086,11 +3164,15 @@
         <v>9.0553851381374173</v>
       </c>
       <c r="H23">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I23">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E24">
         <v>160.30000000000001</v>
       </c>
@@ -3102,11 +3184,15 @@
         <v>7.6811457478686078</v>
       </c>
       <c r="H24">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
-      </c>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I24">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
+      </c>
+    </row>
+    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E25">
         <v>169.3</v>
       </c>
@@ -3118,8 +3204,12 @@
         <v>7</v>
       </c>
       <c r="H25">
-        <f>Stuff!$F$6</f>
-        <v>259</v>
+        <f>Stuff!$I$6</f>
+        <v>51.8</v>
+      </c>
+      <c r="I25">
+        <f>Stuff!$J$6</f>
+        <v>3.2186953878862163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>